<commit_message>
Datadriven Framework-TecStub practical task
</commit_message>
<xml_diff>
--- a/SeleniumJavaFrameWork/Excel/Data.xlsx.xlsx
+++ b/SeleniumJavaFrameWork/Excel/Data.xlsx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,28 +16,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">username </t>
-  </si>
-  <si>
-    <t>varshini</t>
-  </si>
-  <si>
-    <t>password</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Main Menu</t>
+  </si>
+  <si>
+    <t>Sub Menu 1</t>
+  </si>
+  <si>
+    <t>Sub Menu 2</t>
+  </si>
+  <si>
+    <t>Sub Menu 3</t>
+  </si>
+  <si>
+    <t>Domande giudiziali</t>
+  </si>
+  <si>
+    <t>Domande giudiziali 1</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Search in menu</t>
+  </si>
+  <si>
+    <t>Bathroom Furniture</t>
+  </si>
+  <si>
+    <t>HALF
+Sale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,7 +76,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -118,11 +146,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -130,6 +202,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,77 +512,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -510,12 +647,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>